<commit_message>
My last class of Cucumber push
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/HrmsTestData.xlsx
+++ b/src/test/resources/testdata/HrmsTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neilamrami/eclipse-workspace/SyntaxHrms/src/test/resources/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neilamrami/eclipse-workspace/CucumberFrameworkBatch7/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFD5C22-E2FA-D744-A09B-7D71F7727450}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1156605F-B84E-1F44-AEA3-AF2AC061F27E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="4020" windowWidth="14080" windowHeight="15680" xr2:uid="{E54CF63D-5A41-1F4E-A97A-313EF26144AD}"/>
+    <workbookView xWindow="1780" yWindow="3980" windowWidth="14080" windowHeight="15680" xr2:uid="{E54CF63D-5A41-1F4E-A97A-313EF26144AD}"/>
   </bookViews>
   <sheets>
     <sheet name="AddEmployee" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>FirstName</t>
   </si>
@@ -57,34 +57,34 @@
     <t>Doe</t>
   </si>
   <si>
-    <t>Mike</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>Ryan</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
-    <t>Carter</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
     <t>Donald</t>
   </si>
   <si>
     <t>D</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
     <t>Duck</t>
+  </si>
+  <si>
+    <t>Alijon</t>
+  </si>
+  <si>
+    <t>Asel</t>
+  </si>
+  <si>
+    <t>Trump</t>
+  </si>
+  <si>
+    <t>Joe</t>
+  </si>
+  <si>
+    <t>Bidan</t>
+  </si>
+  <si>
+    <t>Employee ID</t>
   </si>
 </sst>
 </file>
@@ -444,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1C1809C-27F4-BD4B-BEB7-438476D35353}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
@@ -455,10 +455,11 @@
     <col min="1" max="1" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,8 +469,11 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -479,49 +483,64 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D2" s="1">
+        <v>222222</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>333333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1">
+        <v>555555</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
+      </c>
+      <c r="D5" s="1">
+        <v>777777</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
+      </c>
+      <c r="D6" s="1">
+        <v>8888888</v>
       </c>
     </row>
   </sheetData>

</xml_diff>